<commit_message>
Added some values in RR02
</commit_message>
<xml_diff>
--- a/TimesheetStorage/TimesheetRR02.xlsx
+++ b/TimesheetStorage/TimesheetRR02.xlsx
@@ -2428,9 +2428,15 @@
           <t>2024-09-15</t>
         </is>
       </c>
-      <c r="C15" s="203" t="n"/>
+      <c r="C15" s="203" t="inlineStr">
+        <is>
+          <t>CQV Shadowing/ PR Document Shadowing and RQ Document Shadowing</t>
+        </is>
+      </c>
       <c r="D15" s="187" t="n"/>
-      <c r="E15" s="204" t="n"/>
+      <c r="E15" s="204" t="n">
+        <v>8</v>
+      </c>
       <c r="F15" s="25" t="n"/>
       <c r="G15" s="201" t="inlineStr">
         <is>
@@ -2525,9 +2531,15 @@
         <f>B15+1</f>
         <v/>
       </c>
-      <c r="C18" s="215" t="n"/>
+      <c r="C18" s="215" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CQV Mapping and Verification Shadowing/ Training for KNEAT and Shadowing/ </t>
+        </is>
+      </c>
       <c r="D18" s="187" t="n"/>
-      <c r="E18" s="204" t="n"/>
+      <c r="E18" s="204" t="n">
+        <v>8</v>
+      </c>
       <c r="F18" s="25" t="n"/>
       <c r="G18" s="201" t="inlineStr">
         <is>

</xml_diff>